<commit_message>
updated grant and teaching info
</commit_message>
<xml_diff>
--- a/RPO_vitae_data.xlsx
+++ b/RPO_vitae_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
   <si>
     <t xml:space="preserve">degree</t>
   </si>
@@ -86,6 +86,18 @@
     <t xml:space="preserve">amount</t>
   </si>
   <si>
+    <t xml:space="preserve">National Taxonomy Research Grant Program (NTGRP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australian Biological Resources Study (ABRS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systematics of Australian mycorrhizal Ceratobasidium (Ceratobasidiaceae)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$20,000</t>
+  </si>
+  <si>
     <t xml:space="preserve">RSB Seed Funding Grant</t>
   </si>
   <si>
@@ -174,6 +186,21 @@
   </si>
   <si>
     <t xml:space="preserve">semester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biology 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIOL1003/BIOL6035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023 S1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Presentation Skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIOL8291</t>
   </si>
   <si>
     <t xml:space="preserve">Data Science for Biologists</t>
@@ -328,24 +355,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -362,7 +393,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -374,73 +405,73 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="52.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -456,102 +487,119 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="48.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="48.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
         <v>2022</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>33</v>
+      <c r="E6" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -566,122 +614,122 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="76.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="76.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="4" t="n">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="n">
         <v>2022</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>2022</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="0" t="n">
+      <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>2022</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>2021</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>2017</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>2017</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="0" t="n">
+      <c r="A8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>2017</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="4" t="n">
+      <c r="A9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3" t="n">
         <v>2016</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="0" t="n">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>2015</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="0" t="n">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>2014</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="0" t="n">
+      <c r="A12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="1" t="n">
         <v>2012</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="0" t="n">
+      <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>2010</v>
       </c>
     </row>
@@ -697,53 +745,75 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>49</v>
+      <c r="A1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>52</v>
+      <c r="A2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>52</v>
+      <c r="A3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -758,133 +828,133 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>56</v>
+      <c r="A1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>58</v>
+      <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>59</v>
+      <c r="A3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>60</v>
+      <c r="A4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>61</v>
+      <c r="A5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>63</v>
+      <c r="A6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>64</v>
+      <c r="A7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>65</v>
+      <c r="A8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>66</v>
+      <c r="A9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>68</v>
+      <c r="A10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>69</v>
+      <c r="A11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>71</v>
+      <c r="A12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>72</v>
+      <c r="A13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>73</v>
+      <c r="A14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated cv - removed non-science stuff
</commit_message>
<xml_diff>
--- a/RPO_vitae_data.xlsx
+++ b/RPO_vitae_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpodonnell/Library/CloudStorage/Dropbox/GitHub/RPO_CV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD26AE2-0D65-ED4A-8B87-7D57745F7388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D7A166-287B-E94E-930A-58F81E865AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="19460" windowHeight="15380" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="19460" windowHeight="15380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="80">
   <si>
     <t>degree</t>
   </si>
@@ -164,30 +164,6 @@
   </si>
   <si>
     <t>University of New England Vice-Chancellor's Scholar</t>
-  </si>
-  <si>
-    <t>Berlin Opera Academy Robert Earl White Memorial Scholarship</t>
-  </si>
-  <si>
-    <t>Berlin Opera Academy Elizabeth Luxon Memorial Scholarship</t>
-  </si>
-  <si>
-    <t>Pacific Opera Young Artist Scholarship</t>
-  </si>
-  <si>
-    <t>Estivo European Chamber Music Summer School Scholarship</t>
-  </si>
-  <si>
-    <t>Best Comedic Film: Tampa Bay Underground Film Festival</t>
-  </si>
-  <si>
-    <t>Best Short Film: Melbourne Underground Film Festival</t>
-  </si>
-  <si>
-    <t>Firstdraft Gallery Emerging Writers Residency</t>
-  </si>
-  <si>
-    <t>University of Sydney Kathleen Garnham Laurence Prize for Fine Arts</t>
   </si>
   <si>
     <t>title</t>
@@ -470,7 +446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -681,10 +657,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B15" sqref="A8:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -746,70 +722,6 @@
       </c>
       <c r="B7">
         <v>2021</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15">
-        <v>2010</v>
       </c>
     </row>
   </sheetData>
@@ -838,57 +750,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -905,7 +817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -918,138 +830,138 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>